<commit_message>
added steps for pushing changes to your branch
</commit_message>
<xml_diff>
--- a/github-command-guide.xlsx
+++ b/github-command-guide.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$23:$C$30</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$42:$C$47</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t xml:space="preserve">Git Commands</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t xml:space="preserve">Push local files to github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steps to push your changes to your working branch on git</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check you are in your local branch</t>
   </si>
   <si>
     <t xml:space="preserve">Steps to get the latest changes from master branch into your local (You should be located in your created off branch)</t>
@@ -176,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -213,6 +219,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -296,7 +307,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -339,6 +350,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -456,15 +471,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C40"/>
+  <dimension ref="A2:C69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="97.22"/>
   </cols>
@@ -601,11 +616,6 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-    </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
         <v>32</v>
@@ -701,9 +711,14 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="7" t="s">
@@ -727,10 +742,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,10 +753,10 @@
         <v>2</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,10 +764,10 @@
         <v>3</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -760,30 +775,171 @@
         <v>4</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="n">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B47" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0"/>
+      <c r="B52" s="0"/>
+      <c r="C52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0"/>
+      <c r="B53" s="0"/>
+      <c r="C53" s="0"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0"/>
+      <c r="B54" s="0"/>
+      <c r="C54" s="0"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0"/>
+      <c r="B55" s="0"/>
+      <c r="C55" s="0"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0"/>
+      <c r="B56" s="0"/>
+      <c r="C56" s="0"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0"/>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0"/>
+      <c r="B58" s="0"/>
+      <c r="C58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0"/>
+      <c r="B59" s="0"/>
+      <c r="C59" s="0"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0"/>
+      <c r="B60" s="0"/>
+      <c r="C60" s="0"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0"/>
+      <c r="B63" s="0"/>
+      <c r="C63" s="0"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0"/>
+      <c r="B64" s="0"/>
+      <c r="C64" s="0"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0"/>
+      <c r="B65" s="0"/>
+      <c r="C65" s="0"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0"/>
+      <c r="B66" s="0"/>
+      <c r="C66" s="0"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0"/>
+      <c r="B67" s="0"/>
+      <c r="C67" s="0"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0"/>
+      <c r="B68" s="0"/>
+      <c r="C68" s="0"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0"/>
+      <c r="B69" s="0"/>
+      <c r="C69" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A23:C30"/>
+  <autoFilter ref="A42:C47"/>
   <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:C4"/>

</xml_diff>